<commit_message>
Improve practice and trial, and several final touches.
</commit_message>
<xml_diff>
--- a/final/conditions.xlsx
+++ b/final/conditions.xlsx
@@ -12,27 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>condition</t>
-  </si>
-  <si>
-    <t>char_1</t>
-  </si>
-  <si>
-    <t>char_2</t>
   </si>
   <si>
     <t>group_name</t>
   </si>
   <si>
     <t>group</t>
-  </si>
-  <si>
-    <t>char_color_1</t>
-  </si>
-  <si>
-    <t>char_color_2</t>
   </si>
   <si>
     <t>color_1</t>
@@ -44,16 +32,10 @@
     <t>agency_level</t>
   </si>
   <si>
-    <t>A</t>
+    <t>Explicit_R</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>explicit</t>
-  </si>
-  <si>
-    <t>yellow</t>
+    <t>green</t>
   </si>
   <si>
     <t>red</t>
@@ -62,55 +44,40 @@
     <t>high</t>
   </si>
   <si>
-    <t>C</t>
+    <t>Implicit_R</t>
   </si>
   <si>
-    <t>implicit</t>
+    <t>purple</t>
   </si>
   <si>
     <t>blue</t>
   </si>
   <si>
-    <t>D</t>
+    <t>Explicit_Free</t>
   </si>
   <si>
-    <t>free</t>
+    <t>low</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>orange</t>
   </si>
   <si>
     <t>white</t>
   </si>
   <si>
-    <t>green</t>
+    <t>Explicit_L</t>
   </si>
   <si>
-    <t>low</t>
+    <t>brown</t>
   </si>
   <si>
-    <t>F</t>
+    <t>Implicit_L</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>invalid</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>purple</t>
-  </si>
-  <si>
-    <t>grey</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>O</t>
+    <t>yellow</t>
   </si>
 </sst>
 </file>
@@ -120,7 +87,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -136,14 +103,8 @@
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
-    <font>
-      <b val="1"/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,12 +114,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -229,19 +184,19 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -264,7 +219,6 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1359,23 +1313,19 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.4" defaultRowHeight="12" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.3516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.3516" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.3516" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.3516" style="1" customWidth="1"/>
-    <col min="11" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.4219" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.4219" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.4219" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.4219" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.4219" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.4219" style="1" customWidth="1"/>
+    <col min="7" max="256" width="16.4219" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.55" customHeight="1">
@@ -1397,49 +1347,25 @@
       <c r="F1" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s" s="2">
-        <v>9</v>
-      </c>
     </row>
     <row r="2" ht="20.55" customHeight="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s" s="4">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
       </c>
       <c r="D2" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="E2" t="s" s="4">
+        <v>8</v>
       </c>
       <c r="F2" t="s" s="4">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s" s="4">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" ht="20.35" customHeight="1">
@@ -1449,29 +1375,17 @@
       <c r="B3" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="C3" t="s" s="6">
-        <v>16</v>
+      <c r="C3" s="5">
+        <v>2</v>
       </c>
       <c r="D3" t="s" s="6">
-        <v>17</v>
-      </c>
-      <c r="E3" s="5">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="E3" t="s" s="6">
+        <v>12</v>
       </c>
       <c r="F3" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s" s="6">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" ht="20.35" customHeight="1">
@@ -1479,31 +1393,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s" s="6">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="C4" s="5">
+        <v>3</v>
       </c>
       <c r="D4" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="E4" s="5">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="E4" t="s" s="6">
+        <v>8</v>
       </c>
       <c r="F4" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="J4" t="s" s="6">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" ht="20.35" customHeight="1">
@@ -1511,415 +1413,1499 @@
         <v>4</v>
       </c>
       <c r="B5" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s" s="6">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4</v>
       </c>
       <c r="D5" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="E5" s="5">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="E5" t="s" s="6">
+        <v>17</v>
       </c>
       <c r="F5" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="I5" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="J5" t="s" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" ht="20.35" customHeight="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s" s="6">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="C6" s="5">
+        <v>5</v>
       </c>
       <c r="D6" t="s" s="6">
-        <v>17</v>
-      </c>
-      <c r="E6" s="5">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="E6" t="s" s="6">
+        <v>19</v>
       </c>
       <c r="F6" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="H6" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="I6" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" ht="20.35" customHeight="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s" s="6">
-        <v>11</v>
+        <v>20</v>
+      </c>
+      <c r="C7" s="5">
+        <v>6</v>
       </c>
       <c r="D7" t="s" s="6">
         <v>12</v>
       </c>
-      <c r="E7" s="5">
-        <v>1</v>
+      <c r="E7" t="s" s="6">
+        <v>16</v>
       </c>
       <c r="F7" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s" s="6">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s" s="6">
-        <v>14</v>
-      </c>
-      <c r="I7" t="s" s="6">
-        <v>14</v>
-      </c>
-      <c r="J7" t="s" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" ht="20.35" customHeight="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s" s="6">
-        <v>25</v>
+        <v>6</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
       </c>
       <c r="D8" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="E8" t="s" s="6">
+        <v>8</v>
       </c>
       <c r="F8" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="G8" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="H8" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="I8" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="J8" t="s" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" ht="20.35" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s" s="6">
         <v>19</v>
       </c>
-      <c r="C9" t="s" s="6">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0</v>
+      <c r="E9" t="s" s="6">
+        <v>12</v>
       </c>
       <c r="F9" t="s" s="6">
-        <v>28</v>
-      </c>
-      <c r="G9" t="s" s="6">
-        <v>29</v>
-      </c>
-      <c r="H9" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="I9" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="J9" t="s" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" ht="20.35" customHeight="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s" s="6">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="C10" s="5">
+        <v>3</v>
       </c>
       <c r="D10" t="s" s="6">
-        <v>12</v>
-      </c>
-      <c r="E10" s="5">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="E10" t="s" s="6">
+        <v>8</v>
       </c>
       <c r="F10" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="G10" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="H10" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="I10" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="J10" t="s" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" ht="20.35" customHeight="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" t="s" s="6">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s" s="6">
-        <v>31</v>
+        <v>15</v>
+      </c>
+      <c r="C11" s="5">
+        <v>4</v>
       </c>
       <c r="D11" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="E11" t="s" s="6">
+        <v>7</v>
       </c>
       <c r="F11" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="G11" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="H11" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="I11" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="J11" t="s" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" ht="20.35" customHeight="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" t="s" s="6">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s" s="6">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="C12" s="5">
+        <v>5</v>
       </c>
       <c r="D12" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="E12" t="s" s="6">
+        <v>21</v>
       </c>
       <c r="F12" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="G12" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="H12" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="I12" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="J12" t="s" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" ht="20.35" customHeight="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" ht="15" customHeight="1">
       <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s" s="6">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="C13" s="5">
+        <v>6</v>
       </c>
       <c r="D13" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="E13" s="5">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="E13" t="s" s="6">
+        <v>17</v>
       </c>
       <c r="F13" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="G13" t="s" s="6">
-        <v>28</v>
-      </c>
-      <c r="H13" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="I13" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="J13" t="s" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" ht="20.35" customHeight="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1">
       <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s" s="6">
         <v>16</v>
       </c>
-      <c r="D14" t="s" s="6">
-        <v>17</v>
-      </c>
-      <c r="E14" s="5">
-        <v>2</v>
+      <c r="E14" t="s" s="6">
+        <v>8</v>
       </c>
       <c r="F14" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="G14" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="H14" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="I14" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="J14" t="s" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" ht="20.35" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" ht="15" customHeight="1">
       <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="C15" t="s" s="6">
-        <v>16</v>
+      <c r="C15" s="5">
+        <v>2</v>
       </c>
       <c r="D15" t="s" s="6">
-        <v>17</v>
-      </c>
-      <c r="E15" s="5">
-        <v>2</v>
+        <v>21</v>
+      </c>
+      <c r="E15" t="s" s="6">
+        <v>12</v>
       </c>
       <c r="F15" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="G15" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="H15" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="I15" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="J15" t="s" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" ht="20.35" customHeight="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" ht="15" customHeight="1">
       <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s" s="6">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="C16" s="5">
+        <v>3</v>
       </c>
       <c r="D16" t="s" s="6">
-        <v>17</v>
-      </c>
-      <c r="E16" s="5">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="E16" t="s" s="6">
+        <v>8</v>
       </c>
       <c r="F16" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="G16" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="H16" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="I16" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="J16" t="s" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" ht="20.35" customHeight="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1">
       <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="C17" s="5">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" ht="15" customHeight="1">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="C18" s="5">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" ht="15" customHeight="1">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="C19" s="5">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" ht="15" customHeight="1">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="E20" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F20" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" ht="15" customHeight="1">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="C17" t="s" s="6">
+      <c r="C21" s="5">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" ht="15" customHeight="1">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="C22" s="5">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F22" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" ht="15" customHeight="1">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="C23" s="5">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="F23" t="s" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" ht="15" customHeight="1">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="C24" s="5">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" ht="15" customHeight="1">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="C25" s="5">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="F25" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" ht="15" customHeight="1">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s" s="6">
         <v>11</v>
       </c>
-      <c r="D17" t="s" s="6">
+      <c r="E26" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F26" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" ht="15" customHeight="1">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="C27" s="5">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="E27" t="s" s="6">
         <v>12</v>
       </c>
-      <c r="E17" s="5">
+      <c r="F27" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" ht="15" customHeight="1">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="C28" s="5">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F28" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" ht="15" customHeight="1">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="C29" s="5">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="F29" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" ht="15" customHeight="1">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="C30" s="5">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="F30" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" ht="15" customHeight="1">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="C31" s="5">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" ht="15" customHeight="1">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="C32" s="5">
         <v>1</v>
       </c>
-      <c r="F17" t="s" s="6">
+      <c r="D32" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" ht="15" customHeight="1">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="C33" s="5">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="F33" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" ht="15" customHeight="1">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s" s="6">
         <v>13</v>
       </c>
-      <c r="G17" t="s" s="6">
+      <c r="C34" s="5">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F34" t="s" s="6">
         <v>14</v>
       </c>
-      <c r="H17" t="s" s="6">
+    </row>
+    <row r="35" ht="15" customHeight="1">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="C35" s="5">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="E35" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="F35" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" ht="15" customHeight="1">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="C36" s="5">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="F36" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" ht="15" customHeight="1">
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="C37" s="5">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" ht="15" customHeight="1">
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="C38" s="5">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="E38" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F38" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" ht="15" customHeight="1">
+      <c r="A39" s="5">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="C39" s="5">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="E39" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="F39" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" ht="15" customHeight="1">
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="C40" s="5">
+        <v>3</v>
+      </c>
+      <c r="D40" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E40" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F40" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" ht="15" customHeight="1">
+      <c r="A41" s="5">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="C41" s="5">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="F41" t="s" s="6">
         <v>14</v>
       </c>
-      <c r="I17" t="s" s="6">
+    </row>
+    <row r="42" ht="15" customHeight="1">
+      <c r="A42" s="5">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="C42" s="5">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E42" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="F42" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" ht="15" customHeight="1">
+      <c r="A43" s="5">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="C43" s="5">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="E43" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="F43" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" ht="15" customHeight="1">
+      <c r="A44" s="5">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="C44" s="5">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="E44" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F44" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" ht="15" customHeight="1">
+      <c r="A45" s="5">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="C45" s="5">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="E45" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="F45" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" ht="15" customHeight="1">
+      <c r="A46" s="5">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="C46" s="5">
+        <v>3</v>
+      </c>
+      <c r="D46" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E46" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F46" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" ht="15" customHeight="1">
+      <c r="A47" s="5">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="C47" s="5">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="E47" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="F47" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" ht="15" customHeight="1">
+      <c r="A48" s="5">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="C48" s="5">
+        <v>5</v>
+      </c>
+      <c r="D48" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E48" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="F48" t="s" s="6">
         <v>14</v>
       </c>
-      <c r="J17" t="s" s="6">
-        <v>23</v>
+    </row>
+    <row r="49" ht="15" customHeight="1">
+      <c r="A49" s="5">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="C49" s="5">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="E49" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="F49" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" ht="15" customHeight="1">
+      <c r="A50" s="5">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="C50" s="5">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="E50" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F50" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" ht="15" customHeight="1">
+      <c r="A51" s="5">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="C51" s="5">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="E51" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="F51" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" ht="15" customHeight="1">
+      <c r="A52" s="5">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="C52" s="5">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E52" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F52" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" ht="15" customHeight="1">
+      <c r="A53" s="5">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="C53" s="5">
+        <v>4</v>
+      </c>
+      <c r="D53" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="E53" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="F53" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" ht="15" customHeight="1">
+      <c r="A54" s="5">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="C54" s="5">
+        <v>5</v>
+      </c>
+      <c r="D54" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E54" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="F54" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" ht="15" customHeight="1">
+      <c r="A55" s="5">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="C55" s="5">
+        <v>6</v>
+      </c>
+      <c r="D55" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="E55" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="F55" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" ht="15" customHeight="1">
+      <c r="A56" s="5">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="C56" s="5">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="E56" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F56" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" ht="15" customHeight="1">
+      <c r="A57" s="5">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="C57" s="5">
+        <v>2</v>
+      </c>
+      <c r="D57" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="E57" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="F57" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" ht="15" customHeight="1">
+      <c r="A58" s="5">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="C58" s="5">
+        <v>3</v>
+      </c>
+      <c r="D58" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E58" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F58" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" ht="15" customHeight="1">
+      <c r="A59" s="5">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="C59" s="5">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="E59" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="F59" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" ht="15" customHeight="1">
+      <c r="A60" s="5">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="C60" s="5">
+        <v>5</v>
+      </c>
+      <c r="D60" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E60" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="F60" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" ht="15" customHeight="1">
+      <c r="A61" s="5">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="C61" s="5">
+        <v>6</v>
+      </c>
+      <c r="D61" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="E61" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="F61" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" ht="15" customHeight="1">
+      <c r="A62" s="5">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="C62" s="5">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="E62" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F62" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" ht="15" customHeight="1">
+      <c r="A63" s="5">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="C63" s="5">
+        <v>2</v>
+      </c>
+      <c r="D63" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="E63" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="F63" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" ht="15" customHeight="1">
+      <c r="A64" s="5">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="C64" s="5">
+        <v>3</v>
+      </c>
+      <c r="D64" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E64" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F64" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" ht="15" customHeight="1">
+      <c r="A65" s="5">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="C65" s="5">
+        <v>4</v>
+      </c>
+      <c r="D65" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="E65" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="F65" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" ht="15" customHeight="1">
+      <c r="A66" s="5">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="C66" s="5">
+        <v>5</v>
+      </c>
+      <c r="D66" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E66" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="F66" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" ht="15" customHeight="1">
+      <c r="A67" s="5">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="C67" s="5">
+        <v>6</v>
+      </c>
+      <c r="D67" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="E67" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="F67" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" ht="15" customHeight="1">
+      <c r="A68" s="5">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="C68" s="5">
+        <v>1</v>
+      </c>
+      <c r="D68" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="E68" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F68" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" ht="15" customHeight="1">
+      <c r="A69" s="5">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="C69" s="5">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="E69" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="F69" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" ht="15" customHeight="1">
+      <c r="A70" s="5">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="C70" s="5">
+        <v>3</v>
+      </c>
+      <c r="D70" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E70" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F70" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" ht="15" customHeight="1">
+      <c r="A71" s="5">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="C71" s="5">
+        <v>4</v>
+      </c>
+      <c r="D71" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="E71" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="F71" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" ht="15" customHeight="1">
+      <c r="A72" s="5">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="C72" s="5">
+        <v>5</v>
+      </c>
+      <c r="D72" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E72" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="F72" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" ht="15" customHeight="1">
+      <c r="A73" s="5">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="C73" s="5">
+        <v>6</v>
+      </c>
+      <c r="D73" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="E73" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="F73" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" ht="15" customHeight="1">
+      <c r="A74" s="5">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="C74" s="5">
+        <v>1</v>
+      </c>
+      <c r="D74" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="E74" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F74" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" ht="15" customHeight="1">
+      <c r="A75" s="5">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="C75" s="5">
+        <v>2</v>
+      </c>
+      <c r="D75" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="E75" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="F75" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" ht="15" customHeight="1">
+      <c r="A76" s="5">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="C76" s="5">
+        <v>3</v>
+      </c>
+      <c r="D76" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E76" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="F76" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" ht="15" customHeight="1">
+      <c r="A77" s="5">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="C77" s="5">
+        <v>4</v>
+      </c>
+      <c r="D77" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="E77" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="F77" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" ht="15" customHeight="1">
+      <c r="A78" s="5">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="C78" s="5">
+        <v>5</v>
+      </c>
+      <c r="D78" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="E78" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="F78" t="s" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" ht="15" customHeight="1">
+      <c r="A79" s="5">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="C79" s="5">
+        <v>6</v>
+      </c>
+      <c r="D79" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="E79" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="F79" t="s" s="6">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve colors, add Tellegen survey data and analysis, improve instructions, and some minor fixes
</commit_message>
<xml_diff>
--- a/final/conditions.xlsx
+++ b/final/conditions.xlsx
@@ -50,7 +50,7 @@
     <t>purple</t>
   </si>
   <si>
-    <t>blue</t>
+    <t>mediumblue</t>
   </si>
   <si>
     <t>Explicit_Free</t>
@@ -104,7 +104,7 @@
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +114,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -187,16 +193,16 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -219,6 +225,7 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>

</xml_diff>

<commit_message>
Update to PychoPy 1.85.2, fix trial colors, and reduce delay (by 0.4s).
</commit_message>
<xml_diff>
--- a/final/conditions.xlsx
+++ b/final/conditions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>condition</t>
   </si>
@@ -47,7 +47,7 @@
     <t>Implicit_R</t>
   </si>
   <si>
-    <t>purple</t>
+    <t>darkviolet</t>
   </si>
   <si>
     <t>mediumblue</t>
@@ -62,7 +62,7 @@
     <t>Control</t>
   </si>
   <si>
-    <t>orange</t>
+    <t>magenta</t>
   </si>
   <si>
     <t>white</t>
@@ -71,13 +71,16 @@
     <t>Explicit_L</t>
   </si>
   <si>
-    <t>brown</t>
+    <t>saddlebrown</t>
   </si>
   <si>
     <t>Implicit_L</t>
   </si>
   <si>
     <t>yellow</t>
+  </si>
+  <si>
+    <t>brown</t>
   </si>
 </sst>
 </file>
@@ -124,7 +127,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -177,13 +180,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -203,6 +236,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1422,10 +1464,10 @@
       <c r="B5" t="s" s="6">
         <v>15</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="7">
         <v>4</v>
       </c>
-      <c r="D5" t="s" s="6">
+      <c r="D5" t="s" s="8">
         <v>16</v>
       </c>
       <c r="E5" t="s" s="6">
@@ -1445,10 +1487,10 @@
       <c r="C6" s="5">
         <v>5</v>
       </c>
-      <c r="D6" t="s" s="6">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s" s="6">
+      <c r="D6" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s" s="8">
         <v>19</v>
       </c>
       <c r="F6" t="s" s="6">
@@ -1465,10 +1507,10 @@
       <c r="C7" s="5">
         <v>6</v>
       </c>
-      <c r="D7" t="s" s="6">
+      <c r="D7" t="s" s="9">
         <v>12</v>
       </c>
-      <c r="E7" t="s" s="6">
+      <c r="E7" t="s" s="8">
         <v>16</v>
       </c>
       <c r="F7" t="s" s="6">
@@ -1502,10 +1544,10 @@
       <c r="B9" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="7">
         <v>2</v>
       </c>
-      <c r="D9" t="s" s="6">
+      <c r="D9" t="s" s="8">
         <v>19</v>
       </c>
       <c r="E9" t="s" s="6">
@@ -1662,10 +1704,10 @@
       <c r="B17" t="s" s="6">
         <v>15</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="7">
         <v>4</v>
       </c>
-      <c r="D17" t="s" s="6">
+      <c r="D17" t="s" s="8">
         <v>19</v>
       </c>
       <c r="E17" t="s" s="6">
@@ -1825,10 +1867,10 @@
       <c r="C25" s="5">
         <v>6</v>
       </c>
-      <c r="D25" t="s" s="6">
+      <c r="D25" t="s" s="9">
         <v>12</v>
       </c>
-      <c r="E25" t="s" s="6">
+      <c r="E25" t="s" s="8">
         <v>19</v>
       </c>
       <c r="F25" t="s" s="6">
@@ -1862,10 +1904,10 @@
       <c r="B27" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="7">
         <v>2</v>
       </c>
-      <c r="D27" t="s" s="6">
+      <c r="D27" t="s" s="8">
         <v>19</v>
       </c>
       <c r="E27" t="s" s="6">
@@ -2029,7 +2071,7 @@
         <v>21</v>
       </c>
       <c r="E35" t="s" s="6">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F35" t="s" s="6">
         <v>9</v>
@@ -2106,7 +2148,7 @@
         <v>2</v>
       </c>
       <c r="D39" t="s" s="6">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E39" t="s" s="6">
         <v>12</v>
@@ -2169,7 +2211,7 @@
         <v>8</v>
       </c>
       <c r="E42" t="s" s="6">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F42" t="s" s="6">
         <v>9</v>
@@ -2266,7 +2308,7 @@
         <v>4</v>
       </c>
       <c r="D47" t="s" s="6">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E47" t="s" s="6">
         <v>21</v>
@@ -2462,10 +2504,10 @@
       <c r="B57" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C57" s="7">
         <v>2</v>
       </c>
-      <c r="D57" t="s" s="6">
+      <c r="D57" t="s" s="8">
         <v>19</v>
       </c>
       <c r="E57" t="s" s="6">
@@ -2745,10 +2787,10 @@
       <c r="C71" s="5">
         <v>4</v>
       </c>
-      <c r="D71" t="s" s="6">
+      <c r="D71" t="s" s="9">
         <v>7</v>
       </c>
-      <c r="E71" t="s" s="6">
+      <c r="E71" t="s" s="8">
         <v>19</v>
       </c>
       <c r="F71" t="s" s="6">
@@ -2822,10 +2864,10 @@
       <c r="B75" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C75" s="7">
         <v>2</v>
       </c>
-      <c r="D75" t="s" s="6">
+      <c r="D75" t="s" s="8">
         <v>19</v>
       </c>
       <c r="E75" t="s" s="6">
@@ -2905,10 +2947,10 @@
       <c r="C79" s="5">
         <v>6</v>
       </c>
-      <c r="D79" t="s" s="6">
+      <c r="D79" t="s" s="9">
         <v>12</v>
       </c>
-      <c r="E79" t="s" s="6">
+      <c r="E79" t="s" s="8">
         <v>19</v>
       </c>
       <c r="F79" t="s" s="6">

</xml_diff>